<commit_message>
Started on inspect_raw.py incorporating early check for null values and at the cups of standardizing text columns.
</commit_message>
<xml_diff>
--- a/project_documentation/gvp_project_structure_and_documentation.xlsx
+++ b/project_documentation/gvp_project_structure_and_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarpy\Documents\portfolio_projects\golden_valley_pipeline\project_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FC2989-5E5B-44CE-B3D5-116BC86D90B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762CEA8C-8E72-493F-8AF9-7D49BC5B0144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4470" windowWidth="20730" windowHeight="11040" xr2:uid="{0C265D32-7742-4C3D-BA88-CDD37B1251D9}"/>
+    <workbookView xWindow="28680" yWindow="4470" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{0C265D32-7742-4C3D-BA88-CDD37B1251D9}"/>
   </bookViews>
   <sheets>
     <sheet name="column_info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>employee_id</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Utility modules that create and update all client folder structure for streamlined setup and editing of client data folders</t>
+  </si>
+  <si>
+    <t>Main Folder</t>
   </si>
 </sst>
 </file>
@@ -587,7 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8E60F5-7BD6-44BF-8BA4-F81BBF6F2092}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -838,10 +841,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9322E22-323C-4169-A3DF-CA21F5C15ECE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -850,7 +864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3329030C-A36F-4B2A-8C4F-757C149DB90B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Completed inspect raw to inspect raw data for nulls and standardize text fields. main_data_io.py has load_raw_data and save_cleaned_data. time_helpers.py contains the completed date, datetime conversion and computations for different lunch and duration times for meal period.
</commit_message>
<xml_diff>
--- a/project_documentation/gvp_project_structure_and_documentation.xlsx
+++ b/project_documentation/gvp_project_structure_and_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarpy\Documents\portfolio_projects\golden_valley_pipeline\project_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762CEA8C-8E72-493F-8AF9-7D49BC5B0144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F367200D-444A-41FD-80BC-6C460E102925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4470" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{0C265D32-7742-4C3D-BA88-CDD37B1251D9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0C265D32-7742-4C3D-BA88-CDD37B1251D9}"/>
   </bookViews>
   <sheets>
     <sheet name="column_info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>employee_id</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>Useful if rest compliance is manually tracked</t>
-  </si>
-  <si>
-    <t>e.g., Full-Time, Part-Time, Temp</t>
   </si>
   <si>
     <t>exempt or non-exempt</t>
@@ -205,6 +202,28 @@
   </si>
   <si>
     <t>Main Folder</t>
+  </si>
+  <si>
+    <t>main_data_io.py</t>
+  </si>
+  <si>
+    <t>1. Incorporated loading of raw data for initial inspection and standardization.
+2. Incorporated saving of cleaned data in processed folder.</t>
+  </si>
+  <si>
+    <t>Expected Format</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD HH:MM:SS</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE</t>
+  </si>
+  <si>
+    <t>e.g., Full-Time, Part-Time, Temp, Seasonal, Contractor</t>
   </si>
 </sst>
 </file>
@@ -588,20 +607,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8E60F5-7BD6-44BF-8BA4-F81BBF6F2092}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="2" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -609,21 +628,24 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -631,10 +653,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -642,10 +667,13 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -653,10 +681,13 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -664,10 +695,13 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -675,10 +709,13 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -686,10 +723,13 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -697,54 +737,57 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -752,10 +795,13 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -763,10 +809,13 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -774,10 +823,13 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -785,51 +837,54 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
-      <c r="C21" t="s">
-        <v>45</v>
+      <c r="D21" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -852,7 +907,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -862,10 +917,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3329030C-A36F-4B2A-8C4F-757C149DB90B}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,16 +934,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -899,10 +954,10 @@
         <v>45878</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -913,10 +968,24 @@
         <v>45878</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>45881</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Figured that the test data were invalid. Gearing up for a rewrite of some methods and assess module integrity.
</commit_message>
<xml_diff>
--- a/project_documentation/gvp_project_structure_and_documentation.xlsx
+++ b/project_documentation/gvp_project_structure_and_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarpy\Documents\portfolio_projects\golden_valley_pipeline\project_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F367200D-444A-41FD-80BC-6C460E102925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA13B614-2110-47C4-B5C3-8C9044395C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0C265D32-7742-4C3D-BA88-CDD37B1251D9}"/>
+    <workbookView xWindow="28680" yWindow="4470" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{0C265D32-7742-4C3D-BA88-CDD37B1251D9}"/>
   </bookViews>
   <sheets>
     <sheet name="column_info" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8E60F5-7BD6-44BF-8BA4-F81BBF6F2092}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -917,10 +917,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3329030C-A36F-4B2A-8C4F-757C149DB90B}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,6 +988,14 @@
         <v>55</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45881</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>